<commit_message>
update to use with the new script
</commit_message>
<xml_diff>
--- a/SafariWhiteList.xlsx
+++ b/SafariWhiteList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Niels/Dropbox/UCB/Scriptz/SafariWhiteList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84D6546D-24B6-7641-9112-585C7927B8AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D912DFC-2B24-024C-86F3-B382BAD952FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16980" yWindow="-21140" windowWidth="19200" windowHeight="21140" xr2:uid="{980CFCA4-16E9-B144-B743-1B53827CD32B}"/>
   </bookViews>
@@ -31,36 +31,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Requested_value</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://surveys.healthvibe.eu</t>
-  </si>
-  <si>
-    <t>surveys.healthvibe.eu</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>google.be</t>
   </si>
   <si>
     <t>https://google.be</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>https://facebook.be</t>
+  </si>
+  <si>
+    <t>REQ</t>
+  </si>
+  <si>
+    <t>VAL</t>
+  </si>
+  <si>
+    <t>siteURL</t>
+  </si>
+  <si>
+    <t>justavalue</t>
   </si>
 </sst>
 </file>
@@ -423,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2351CB8A-78A6-3447-9344-410E124253C2}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,29 +431,32 @@
     <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -464,35 +464,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{D4F2CBED-C6C7-E948-8823-9F1B966B8B9A}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{39E023B3-AE6D-0841-BE69-19DD45194F99}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{8C37DCD4-C854-4E42-B53C-6492E6936720}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{6D609D5E-8F47-3F4A-B68D-1C4D58851230}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>